<commit_message>
Fix for configurations that have wrong deployed date
</commit_message>
<xml_diff>
--- a/Configurations/CM_1.0.4_21022019.xlsx
+++ b/Configurations/CM_1.0.4_21022019.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming Yu\Documents\SMU\IS214\transfer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ming Yu\Documents\SMU\IS214\esm214\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD0DC7B-F543-4062-8CA9-AF9DF394421A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1434703-F0B2-43AA-942E-E80718148A30}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{2BB56906-853E-4336-8E30-9BAFB26AF772}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="45">
-  <si>
-    <t>Date Deployed: 18/2/2019</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Deployment Environment</t>
   </si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>8000-8999</t>
+  </si>
+  <si>
+    <t>Date Deployed: 21/2/2019</t>
   </si>
 </sst>
 </file>
@@ -718,9 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93682F7B-66A1-4A6C-AA5E-0430957AF32E}">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
   <cols>
@@ -731,7 +729,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B1" s="2"/>
     </row>
@@ -745,10 +743,10 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1">
@@ -757,15 +755,15 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="4">
         <v>1</v>
@@ -773,7 +771,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="4">
         <v>1</v>
@@ -781,137 +779,137 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1">
       <c r="A9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1">
       <c r="A20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="11"/>
       <c r="B26" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>34</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="10"/>
       <c r="B31" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="11"/>
       <c r="B32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" s="12">
         <v>8000</v>
@@ -950,33 +948,33 @@
     <row r="40" spans="1:2">
       <c r="A40" s="19"/>
       <c r="B40" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="10"/>
       <c r="B43" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="10"/>
       <c r="B44" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="11"/>
       <c r="B45" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>